<commit_message>
add -i option, emend README
</commit_message>
<xml_diff>
--- a/box.xlsx
+++ b/box.xlsx
@@ -2335,73 +2335,73 @@
     <t>2017-09-22</t>
   </si>
   <si>
+    <t>2017-05-12</t>
+  </si>
+  <si>
+    <t>2017-07-07</t>
+  </si>
+  <si>
+    <t>2017-08-24</t>
+  </si>
+  <si>
+    <t>2016-11-18</t>
+  </si>
+  <si>
+    <t>2017-04-19</t>
+  </si>
+  <si>
+    <t>2017-08-04</t>
+  </si>
+  <si>
+    <t>2016-11-12</t>
+  </si>
+  <si>
+    <t>2016-12-02</t>
+  </si>
+  <si>
+    <t>2017-04-14</t>
+  </si>
+  <si>
+    <t>2017-06-23</t>
+  </si>
+  <si>
+    <t>2017-04-24</t>
+  </si>
+  <si>
+    <t>2016-12-30</t>
+  </si>
+  <si>
+    <t>2017-06-09</t>
+  </si>
+  <si>
+    <t>2017-09-18</t>
+  </si>
+  <si>
+    <t>2017-07-24</t>
+  </si>
+  <si>
+    <t>2017-05-26</t>
+  </si>
+  <si>
+    <t>2017-09-28</t>
+  </si>
+  <si>
+    <t>2017-03-12</t>
+  </si>
+  <si>
+    <t>2017-06-06</t>
+  </si>
+  <si>
+    <t>2017-03-20</t>
+  </si>
+  <si>
+    <t>2017-06-10</t>
+  </si>
+  <si>
+    <t>2016-12-26</t>
+  </si>
+  <si>
     <t>2017-08-28</t>
-  </si>
-  <si>
-    <t>2017-05-12</t>
-  </si>
-  <si>
-    <t>2017-07-07</t>
-  </si>
-  <si>
-    <t>2017-08-24</t>
-  </si>
-  <si>
-    <t>2016-11-18</t>
-  </si>
-  <si>
-    <t>2017-04-19</t>
-  </si>
-  <si>
-    <t>2017-08-04</t>
-  </si>
-  <si>
-    <t>2016-11-12</t>
-  </si>
-  <si>
-    <t>2016-12-02</t>
-  </si>
-  <si>
-    <t>2017-04-14</t>
-  </si>
-  <si>
-    <t>2017-06-23</t>
-  </si>
-  <si>
-    <t>2017-04-24</t>
-  </si>
-  <si>
-    <t>2016-12-30</t>
-  </si>
-  <si>
-    <t>2017-06-09</t>
-  </si>
-  <si>
-    <t>2017-09-18</t>
-  </si>
-  <si>
-    <t>2017-07-24</t>
-  </si>
-  <si>
-    <t>2017-05-26</t>
-  </si>
-  <si>
-    <t>2017-09-28</t>
-  </si>
-  <si>
-    <t>2017-03-12</t>
-  </si>
-  <si>
-    <t>2017-06-06</t>
-  </si>
-  <si>
-    <t>2017-03-20</t>
-  </si>
-  <si>
-    <t>2017-06-10</t>
-  </si>
-  <si>
-    <t>2016-12-26</t>
   </si>
   <si>
     <t>2016-12-19</t>
@@ -7823,16 +7823,16 @@
     </row>
     <row r="132" spans="1:12">
       <c r="A132" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C132">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D132">
-        <v>104</v>
+        <v>56</v>
       </c>
       <c r="E132" t="s">
         <v>38</v>
@@ -7841,22 +7841,22 @@
         <v>211</v>
       </c>
       <c r="G132" t="s">
-        <v>773</v>
+        <v>726</v>
       </c>
       <c r="H132">
+        <v>56</v>
+      </c>
+      <c r="I132">
         <v>39</v>
       </c>
-      <c r="I132">
-        <v>38</v>
-      </c>
       <c r="J132">
-        <v>27774</v>
+        <v>28000</v>
       </c>
       <c r="K132">
-        <v>6394779</v>
+        <v>6445649</v>
       </c>
       <c r="L132" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:12">
@@ -7917,7 +7917,7 @@
         <v>213</v>
       </c>
       <c r="G134" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H134">
         <v>91</v>
@@ -8069,7 +8069,7 @@
         <v>217</v>
       </c>
       <c r="G138" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H138">
         <v>64</v>
@@ -8183,7 +8183,7 @@
         <v>220</v>
       </c>
       <c r="G141" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="H141">
         <v>36</v>
@@ -8221,7 +8221,7 @@
         <v>221</v>
       </c>
       <c r="G142" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H142">
         <v>71</v>
@@ -8449,7 +8449,7 @@
         <v>227</v>
       </c>
       <c r="G148" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="H148">
         <v>54</v>
@@ -8525,7 +8525,7 @@
         <v>229</v>
       </c>
       <c r="G150" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H150">
         <v>81</v>
@@ -8715,7 +8715,7 @@
         <v>234</v>
       </c>
       <c r="G155" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="H155">
         <v>45</v>
@@ -8829,7 +8829,7 @@
         <v>237</v>
       </c>
       <c r="G158" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H158">
         <v>57</v>
@@ -8943,7 +8943,7 @@
         <v>240</v>
       </c>
       <c r="G161" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H161">
         <v>49</v>
@@ -8981,7 +8981,7 @@
         <v>241</v>
       </c>
       <c r="G162" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H162">
         <v>38</v>
@@ -9171,7 +9171,7 @@
         <v>246</v>
       </c>
       <c r="G167" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H167">
         <v>73</v>
@@ -9209,7 +9209,7 @@
         <v>247</v>
       </c>
       <c r="G168" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H168">
         <v>35</v>
@@ -9589,7 +9589,7 @@
         <v>257</v>
       </c>
       <c r="G178" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H178">
         <v>70</v>
@@ -9665,7 +9665,7 @@
         <v>259</v>
       </c>
       <c r="G180" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H180">
         <v>40</v>
@@ -9703,7 +9703,7 @@
         <v>260</v>
       </c>
       <c r="G181" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H181">
         <v>49</v>
@@ -9817,7 +9817,7 @@
         <v>263</v>
       </c>
       <c r="G184" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H184">
         <v>32</v>
@@ -9855,7 +9855,7 @@
         <v>264</v>
       </c>
       <c r="G185" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H185">
         <v>28</v>
@@ -10007,7 +10007,7 @@
         <v>268</v>
       </c>
       <c r="G189" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H189">
         <v>39</v>
@@ -10311,7 +10311,7 @@
         <v>276</v>
       </c>
       <c r="G197" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H197">
         <v>47</v>
@@ -10349,7 +10349,7 @@
         <v>277</v>
       </c>
       <c r="G198" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H198">
         <v>37</v>
@@ -10539,7 +10539,7 @@
         <v>282</v>
       </c>
       <c r="G203" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H203">
         <v>45</v>
@@ -10729,7 +10729,7 @@
         <v>287</v>
       </c>
       <c r="G208" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H208">
         <v>42</v>
@@ -10767,7 +10767,7 @@
         <v>288</v>
       </c>
       <c r="G209" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H209">
         <v>38</v>
@@ -10843,7 +10843,7 @@
         <v>290</v>
       </c>
       <c r="G211" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H211">
         <v>60</v>
@@ -10995,7 +10995,7 @@
         <v>294</v>
       </c>
       <c r="G215" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H215">
         <v>36</v>
@@ -11261,7 +11261,7 @@
         <v>301</v>
       </c>
       <c r="G222" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="H222">
         <v>44</v>
@@ -11451,7 +11451,7 @@
         <v>306</v>
       </c>
       <c r="G227" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H227">
         <v>59</v>
@@ -11489,7 +11489,7 @@
         <v>307</v>
       </c>
       <c r="G228" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H228">
         <v>29</v>
@@ -11603,7 +11603,7 @@
         <v>310</v>
       </c>
       <c r="G231" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H231">
         <v>28</v>
@@ -11641,7 +11641,7 @@
         <v>311</v>
       </c>
       <c r="G232" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H232">
         <v>55</v>
@@ -11755,7 +11755,7 @@
         <v>314</v>
       </c>
       <c r="G235" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H235">
         <v>21</v>
@@ -11831,7 +11831,7 @@
         <v>316</v>
       </c>
       <c r="G237" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H237">
         <v>52</v>
@@ -12021,7 +12021,7 @@
         <v>321</v>
       </c>
       <c r="G242" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="H242">
         <v>27</v>
@@ -12249,7 +12249,7 @@
         <v>327</v>
       </c>
       <c r="G248" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H248">
         <v>16</v>
@@ -12439,7 +12439,7 @@
         <v>332</v>
       </c>
       <c r="G253" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H253">
         <v>34</v>
@@ -12515,7 +12515,7 @@
         <v>334</v>
       </c>
       <c r="G255" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H255">
         <v>29</v>
@@ -12553,7 +12553,7 @@
         <v>335</v>
       </c>
       <c r="G256" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H256">
         <v>38</v>
@@ -12743,7 +12743,7 @@
         <v>340</v>
       </c>
       <c r="G261" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="H261">
         <v>5</v>
@@ -12819,7 +12819,7 @@
         <v>342</v>
       </c>
       <c r="G263" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H263">
         <v>13</v>
@@ -12857,7 +12857,7 @@
         <v>343</v>
       </c>
       <c r="G264" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="H264">
         <v>29</v>
@@ -13123,7 +13123,7 @@
         <v>350</v>
       </c>
       <c r="G271" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H271">
         <v>38</v>
@@ -13275,7 +13275,7 @@
         <v>354</v>
       </c>
       <c r="G275" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H275">
         <v>49</v>
@@ -13579,7 +13579,7 @@
         <v>362</v>
       </c>
       <c r="G283" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H283">
         <v>27</v>
@@ -13693,7 +13693,7 @@
         <v>365</v>
       </c>
       <c r="G286" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H286">
         <v>50</v>
@@ -13807,7 +13807,7 @@
         <v>368</v>
       </c>
       <c r="G289" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H289">
         <v>31</v>
@@ -13883,7 +13883,7 @@
         <v>370</v>
       </c>
       <c r="G291" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H291">
         <v>21</v>
@@ -13921,7 +13921,7 @@
         <v>371</v>
       </c>
       <c r="G292" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H292">
         <v>25</v>
@@ -13959,7 +13959,7 @@
         <v>372</v>
       </c>
       <c r="G293" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H293">
         <v>34</v>
@@ -14073,7 +14073,7 @@
         <v>375</v>
       </c>
       <c r="G296" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H296">
         <v>88</v>
@@ -14187,7 +14187,7 @@
         <v>378</v>
       </c>
       <c r="G299" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H299">
         <v>50</v>
@@ -14301,7 +14301,7 @@
         <v>381</v>
       </c>
       <c r="G302" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H302">
         <v>29</v>
@@ -14491,7 +14491,7 @@
         <v>386</v>
       </c>
       <c r="G307" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H307">
         <v>21</v>
@@ -14529,7 +14529,7 @@
         <v>387</v>
       </c>
       <c r="G308" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H308">
         <v>25</v>
@@ -14719,7 +14719,7 @@
         <v>392</v>
       </c>
       <c r="G313" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H313">
         <v>27</v>
@@ -14833,7 +14833,7 @@
         <v>395</v>
       </c>
       <c r="G316" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H316">
         <v>24</v>
@@ -15023,7 +15023,7 @@
         <v>400</v>
       </c>
       <c r="G321" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H321">
         <v>14</v>
@@ -15175,7 +15175,7 @@
         <v>404</v>
       </c>
       <c r="G325" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H325">
         <v>42</v>
@@ -15213,7 +15213,7 @@
         <v>405</v>
       </c>
       <c r="G326" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H326">
         <v>36</v>
@@ -15479,7 +15479,7 @@
         <v>412</v>
       </c>
       <c r="G333" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H333">
         <v>22</v>
@@ -15707,7 +15707,7 @@
         <v>418</v>
       </c>
       <c r="G339" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H339">
         <v>22</v>
@@ -15783,7 +15783,7 @@
         <v>420</v>
       </c>
       <c r="G341" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H341">
         <v>14</v>
@@ -15973,7 +15973,7 @@
         <v>425</v>
       </c>
       <c r="G346" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H346">
         <v>14</v>
@@ -16125,7 +16125,7 @@
         <v>429</v>
       </c>
       <c r="G350" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H350">
         <v>21</v>
@@ -16201,7 +16201,7 @@
         <v>431</v>
       </c>
       <c r="G352" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H352">
         <v>35</v>
@@ -16239,7 +16239,7 @@
         <v>432</v>
       </c>
       <c r="G353" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H353">
         <v>22</v>
@@ -16619,7 +16619,7 @@
         <v>442</v>
       </c>
       <c r="G363" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H363">
         <v>20</v>
@@ -16657,7 +16657,7 @@
         <v>443</v>
       </c>
       <c r="G364" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H364">
         <v>15</v>
@@ -16733,7 +16733,7 @@
         <v>445</v>
       </c>
       <c r="G366" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H366">
         <v>16</v>
@@ -17303,7 +17303,7 @@
         <v>460</v>
       </c>
       <c r="G381" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H381">
         <v>18</v>
@@ -17493,7 +17493,7 @@
         <v>465</v>
       </c>
       <c r="G386" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H386">
         <v>42</v>
@@ -17683,7 +17683,7 @@
         <v>470</v>
       </c>
       <c r="G391" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H391">
         <v>14</v>
@@ -17797,7 +17797,7 @@
         <v>473</v>
       </c>
       <c r="G394" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H394">
         <v>14</v>
@@ -17835,7 +17835,7 @@
         <v>474</v>
       </c>
       <c r="G395" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H395">
         <v>13</v>
@@ -17949,7 +17949,7 @@
         <v>477</v>
       </c>
       <c r="G398" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="H398">
         <v>25</v>
@@ -17987,7 +17987,7 @@
         <v>478</v>
       </c>
       <c r="G399" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H399">
         <v>17</v>
@@ -18177,7 +18177,7 @@
         <v>483</v>
       </c>
       <c r="G404" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H404">
         <v>14</v>
@@ -18367,7 +18367,7 @@
         <v>488</v>
       </c>
       <c r="G409" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H409">
         <v>17</v>
@@ -18443,7 +18443,7 @@
         <v>490</v>
       </c>
       <c r="G411" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H411">
         <v>14</v>
@@ -18557,7 +18557,7 @@
         <v>493</v>
       </c>
       <c r="G414" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H414">
         <v>14</v>
@@ -18633,7 +18633,7 @@
         <v>495</v>
       </c>
       <c r="G416" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H416">
         <v>15</v>
@@ -19051,7 +19051,7 @@
         <v>506</v>
       </c>
       <c r="G427" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="H427">
         <v>4</v>
@@ -19203,7 +19203,7 @@
         <v>510</v>
       </c>
       <c r="G431" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H431">
         <v>14</v>
@@ -19355,7 +19355,7 @@
         <v>514</v>
       </c>
       <c r="G435" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H435">
         <v>18</v>
@@ -19431,7 +19431,7 @@
         <v>516</v>
       </c>
       <c r="G437" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H437">
         <v>14</v>
@@ -19583,7 +19583,7 @@
         <v>520</v>
       </c>
       <c r="G441" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H441">
         <v>14</v>
@@ -19811,7 +19811,7 @@
         <v>526</v>
       </c>
       <c r="G447" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H447">
         <v>14</v>
@@ -20533,7 +20533,7 @@
         <v>545</v>
       </c>
       <c r="G466" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="H466">
         <v>11</v>
@@ -20837,7 +20837,7 @@
         <v>553</v>
       </c>
       <c r="G474" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H474">
         <v>14</v>
@@ -20989,7 +20989,7 @@
         <v>557</v>
       </c>
       <c r="G478" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H478">
         <v>12</v>
@@ -21065,7 +21065,7 @@
         <v>559</v>
       </c>
       <c r="G480" t="s">
-        <v>773</v>
+        <v>795</v>
       </c>
       <c r="H480">
         <v>9</v>
@@ -21179,7 +21179,7 @@
         <v>562</v>
       </c>
       <c r="G483" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H483">
         <v>18</v>
@@ -21559,7 +21559,7 @@
         <v>572</v>
       </c>
       <c r="G493" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H493">
         <v>14</v>
@@ -21673,7 +21673,7 @@
         <v>575</v>
       </c>
       <c r="G496" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="H496">
         <v>23</v>
@@ -21711,7 +21711,7 @@
         <v>576</v>
       </c>
       <c r="G497" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H497">
         <v>7</v>
@@ -21787,7 +21787,7 @@
         <v>578</v>
       </c>
       <c r="G499" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H499">
         <v>14</v>
@@ -22015,7 +22015,7 @@
         <v>584</v>
       </c>
       <c r="G505" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="H505">
         <v>12</v>
@@ -22509,7 +22509,7 @@
         <v>597</v>
       </c>
       <c r="G518" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="H518">
         <v>13</v>
@@ -23041,7 +23041,7 @@
         <v>611</v>
       </c>
       <c r="G532" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="H532">
         <v>21</v>
@@ -24029,7 +24029,7 @@
         <v>637</v>
       </c>
       <c r="G558" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H558">
         <v>3</v>
@@ -24067,7 +24067,7 @@
         <v>638</v>
       </c>
       <c r="G559" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H559">
         <v>3</v>
@@ -24181,7 +24181,7 @@
         <v>641</v>
       </c>
       <c r="G562" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="H562">
         <v>12</v>
@@ -24409,7 +24409,7 @@
         <v>647</v>
       </c>
       <c r="G568" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H568">
         <v>7</v>
@@ -24561,7 +24561,7 @@
         <v>651</v>
       </c>
       <c r="G572" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H572">
         <v>2</v>
@@ -24675,7 +24675,7 @@
         <v>654</v>
       </c>
       <c r="G575" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H575">
         <v>5</v>
@@ -24827,7 +24827,7 @@
         <v>658</v>
       </c>
       <c r="G579" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="H579">
         <v>2</v>
@@ -25131,7 +25131,7 @@
         <v>666</v>
       </c>
       <c r="G587" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H587">
         <v>5</v>
@@ -25207,7 +25207,7 @@
         <v>668</v>
       </c>
       <c r="G589" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="H589">
         <v>2</v>
@@ -25245,7 +25245,7 @@
         <v>669</v>
       </c>
       <c r="G590" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H590">
         <v>4</v>
@@ -25321,7 +25321,7 @@
         <v>671</v>
       </c>
       <c r="G592" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H592">
         <v>4</v>
@@ -25397,7 +25397,7 @@
         <v>673</v>
       </c>
       <c r="G594" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="H594">
         <v>3</v>
@@ -25625,7 +25625,7 @@
         <v>679</v>
       </c>
       <c r="G600" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="H600">
         <v>3</v>
@@ -25663,7 +25663,7 @@
         <v>680</v>
       </c>
       <c r="G601" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="H601">
         <v>3</v>
@@ -26233,7 +26233,7 @@
         <v>695</v>
       </c>
       <c r="G616" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="H616">
         <v>3</v>

</xml_diff>